<commit_message>
整理注释 add by songxzh 20180906
</commit_message>
<xml_diff>
--- a/2018-2019plan.xlsx
+++ b/2018-2019plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\terry\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{314F0D30-554E-48CF-A173-96F7345DD4F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6B7E26CD-681C-4174-90AC-5BDC9FF1F986}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10390" activeTab="2" xr2:uid="{992D1F4C-7EB5-409F-99F6-499B88E99E0D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10392" activeTab="2" xr2:uid="{992D1F4C-7EB5-409F-99F6-499B88E99E0D}"/>
   </bookViews>
   <sheets>
     <sheet name="方针" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="一览表-9月" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -134,6 +133,462 @@
           </rPr>
           <t xml:space="preserve">
 日常表现积极；不打架、不骂人；适当奖励一朵红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{4DD8CCF9-E84A-45A0-987A-AFD9F572730F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+主动帮助别人干活；和他人分享自己的东西；适当奖励一朵红花。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{06AE59C2-8BBD-414D-ABFC-E305BDE4F55F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+主动看书、学习知识；奖励一朵红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{FBF69898-A788-47C8-B278-AA72BD9477C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+英语课上，老师给与表扬（得分超过25），给与一朵红花奖励。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{496815C5-0F73-4F26-BCBE-C71232BE5863}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+学校里，老师给与口头或书面夸奖后，奖励一朵红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{91DAEB54-F6EC-46BE-A04B-648D75BDAA92}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+主动正确完成，并提前提交英语作业，奖励一朵红花；超额完成作业，补加奖励一朵红花。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{1D0F54F3-CE5B-4F92-8B96-E30E633D65F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+每一次认识5个新的生字（汉语或英文），奖励一朵红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{8792CBCA-2430-44FE-814E-D5B40140B58F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+每周能背诵并讲解一首古诗，奖励三（2+1）朵红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{9E513EE5-F147-490F-B05D-20C7CA8ED5DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+每能背诵10句三字经，奖励一朵红花。（不计重复背诵）</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{7B71BC1A-7455-498E-B56C-3536C224A524}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+每能主动讲解一个小故事，奖励两朵红花。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{229AEEC9-5BFD-4DF4-B6D3-30928EF95677}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+每日能主动跟家人分享学校生活、学习，适当奖励一朵红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{0DEC97BA-E0DE-42AD-B141-1FAE68AAB4C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+如果能说服别人接受自己观点，并过说服人同意，奖励一朵红花。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{AA3D56F4-3C7D-4AB4-A72C-D6B7875C58D8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+主动做出周计划，并按照计划完成80%以上，奖励五朵小红花。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{39F2B409-5713-450C-8A58-8E8F53CEE074}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+早上懒床，不主动洗漱；上学迟到（8：10）；扣减一朵红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{EF144D3F-8732-4FE2-92A4-1F37974F4B01}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+晚上9：30未上床，或10：30前未睡觉；扣减一朵红花；</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{00BD1DAF-958D-4C42-A259-6C2F8781ED6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+打架、骂人、摔东西；扣减一朵小红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{829E3BB7-00A1-4323-947B-BFA6C4DD8562}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+连续看电视40分钟以上；扣减一朵小红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{A49BF940-82A3-4A3D-B83A-05266D0A4A0D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+玩过的玩具，不主动收拾；扣减一朵小红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{6931543F-9B2F-4EA1-AB70-286A1C333B1D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+饭前不洗手，扣减一朵小红花</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{D4E6E86D-17DF-42AE-B887-13B7D981E449}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>terry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+学校老师提出批评，扣减两朵小红花</t>
         </r>
       </text>
     </comment>
@@ -611,7 +1066,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +1111,19 @@
       <color indexed="81"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -807,19 +1275,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -866,6 +1322,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,22 +1655,22 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1210,62 +1678,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>15</v>
       </c>
@@ -1281,23 +1749,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E969F821-CC18-45B3-A76E-178B6A930C5D}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -1305,7 +1773,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1781,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1321,12 +1789,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1334,7 +1802,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1342,7 +1810,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1350,12 +1818,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -1363,7 +1831,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -1371,7 +1839,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
@@ -1379,7 +1847,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>29</v>
       </c>
@@ -1387,7 +1855,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>30</v>
       </c>
@@ -1395,7 +1863,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>31</v>
       </c>
@@ -1403,7 +1871,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>32</v>
       </c>
@@ -1411,7 +1879,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>33</v>
       </c>
@@ -1419,7 +1887,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -1427,7 +1895,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>35</v>
       </c>
@@ -1435,17 +1903,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>37</v>
       </c>
@@ -1453,7 +1921,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -1461,17 +1929,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>40</v>
       </c>
@@ -1479,7 +1947,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>41</v>
       </c>
@@ -1487,7 +1955,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>42</v>
       </c>
@@ -1495,7 +1963,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>43</v>
       </c>
@@ -1503,12 +1971,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>44</v>
       </c>
@@ -1516,22 +1984,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>50</v>
       </c>
@@ -1539,7 +2007,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>100</v>
       </c>
@@ -1547,7 +2015,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>200</v>
       </c>
@@ -1555,7 +2023,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>500</v>
       </c>
@@ -1563,7 +2031,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>1000</v>
       </c>
@@ -1582,1330 +2050,1330 @@
   <dimension ref="B1:AI32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL17" sqref="AL17"/>
+      <selection activeCell="AK22" sqref="AK22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="35" width="3.08203125" customWidth="1"/>
+    <col min="5" max="35" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21">
         <v>43344</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-    </row>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="10">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="20"/>
+    </row>
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="6">
         <v>2</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="4">
         <v>3</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="4">
         <v>4</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="4">
         <v>5</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="4">
         <v>6</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="4">
         <v>7</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="6">
         <v>8</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="6">
         <v>9</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="4">
         <v>10</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="4">
         <v>11</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="4">
         <v>12</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="4">
         <v>13</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="4">
         <v>14</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="6">
         <v>15</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="6">
         <v>16</v>
       </c>
-      <c r="U2" s="7">
+      <c r="U2" s="4">
         <v>17</v>
       </c>
-      <c r="V2" s="7">
+      <c r="V2" s="4">
         <v>18</v>
       </c>
-      <c r="W2" s="7">
+      <c r="W2" s="4">
         <v>19</v>
       </c>
-      <c r="X2" s="7">
+      <c r="X2" s="4">
         <v>20</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="Y2" s="4">
         <v>21</v>
       </c>
-      <c r="Z2" s="10">
+      <c r="Z2" s="6">
         <v>22</v>
       </c>
-      <c r="AA2" s="10">
+      <c r="AA2" s="6">
         <v>23</v>
       </c>
-      <c r="AB2" s="7">
+      <c r="AB2" s="4">
         <v>24</v>
       </c>
-      <c r="AC2" s="7">
+      <c r="AC2" s="4">
         <v>25</v>
       </c>
-      <c r="AD2" s="7">
+      <c r="AD2" s="4">
         <v>26</v>
       </c>
-      <c r="AE2" s="7">
+      <c r="AE2" s="4">
         <v>27</v>
       </c>
-      <c r="AF2" s="7">
+      <c r="AF2" s="4">
         <v>28</v>
       </c>
-      <c r="AG2" s="10">
+      <c r="AG2" s="6">
         <v>29</v>
       </c>
-      <c r="AH2" s="10">
+      <c r="AH2" s="6">
         <v>30</v>
       </c>
-      <c r="AI2" s="7"/>
-    </row>
-    <row r="3" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="AI2" s="4"/>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="22" t="s">
         <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
       <c r="AI3" s="2"/>
     </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
       <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
       <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="22"/>
-    </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="18"/>
+    </row>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="22"/>
-      <c r="AE7" s="22"/>
-      <c r="AF7" s="22"/>
-      <c r="AG7" s="11"/>
-      <c r="AH7" s="11"/>
-      <c r="AI7" s="22"/>
-    </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="18"/>
+    </row>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="22"/>
-    </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="18"/>
+    </row>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22" t="s">
         <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
-      <c r="AG9" s="11"/>
-      <c r="AH9" s="11"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
       <c r="AI9" s="2"/>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="11"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
       <c r="AI10" s="2"/>
     </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
       <c r="AI11" s="2"/>
     </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
       <c r="AI12" s="2"/>
     </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
       <c r="AI13" s="2"/>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
       <c r="AI14" s="2"/>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
       <c r="AI15" s="2"/>
     </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
       <c r="AI16" s="2"/>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+    <row r="17" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
       <c r="AI17" s="2"/>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+    <row r="18" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="11"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
       <c r="AI18" s="2"/>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="16">
+    <row r="19" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="12">
         <f>SUM(E3:E18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="16">
-        <f t="shared" ref="F19:AI19" si="0">SUM(F3:F18)</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="16">
+      <c r="F19" s="12">
+        <f t="shared" ref="F19:AH19" si="0">SUM(F3:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N19" s="16">
+      <c r="N19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P19" s="16">
+      <c r="P19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="16">
+      <c r="Q19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S19" s="16">
+      <c r="S19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T19" s="16">
+      <c r="T19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U19" s="16">
+      <c r="U19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V19" s="16">
+      <c r="V19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W19" s="16">
+      <c r="W19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X19" s="16">
+      <c r="X19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="16">
+      <c r="Y19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z19" s="16">
+      <c r="Z19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA19" s="16">
+      <c r="AA19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB19" s="16">
+      <c r="AB19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC19" s="16">
+      <c r="AC19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD19" s="16">
+      <c r="AD19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE19" s="16">
+      <c r="AE19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF19" s="16">
+      <c r="AF19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AG19" s="16">
+      <c r="AG19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AH19" s="16">
+      <c r="AH19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AI19" s="17"/>
-    </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="18"/>
-      <c r="AB20" s="18"/>
-      <c r="AC20" s="18"/>
-      <c r="AD20" s="18"/>
-      <c r="AE20" s="18"/>
-      <c r="AF20" s="18"/>
-      <c r="AG20" s="18"/>
-      <c r="AH20" s="18"/>
-      <c r="AI20" s="19"/>
-    </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B21" s="8" t="s">
+      <c r="AI19" s="13"/>
+    </row>
+    <row r="20" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="14"/>
+      <c r="AG20" s="14"/>
+      <c r="AH20" s="14"/>
+      <c r="AI20" s="15"/>
+    </row>
+    <row r="21" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="11"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
-      <c r="AG21" s="11"/>
-      <c r="AH21" s="11"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
       <c r="AI21" s="2"/>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9" t="s">
+    <row r="22" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
+      <c r="AG22" s="7"/>
+      <c r="AH22" s="7"/>
       <c r="AI22" s="2"/>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8" t="s">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B23" s="23"/>
+      <c r="C23" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="23"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="23"/>
-      <c r="AC23" s="23"/>
-      <c r="AD23" s="23"/>
-      <c r="AE23" s="23"/>
-      <c r="AF23" s="23"/>
-      <c r="AG23" s="11"/>
-      <c r="AH23" s="11"/>
-      <c r="AI23" s="23"/>
-    </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9" t="s">
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="19"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="19"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19"/>
+      <c r="AF23" s="19"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="19"/>
+    </row>
+    <row r="24" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="23"/>
-      <c r="X24" s="23"/>
-      <c r="Y24" s="23"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="23"/>
-      <c r="AC24" s="23"/>
-      <c r="AD24" s="23"/>
-      <c r="AE24" s="23"/>
-      <c r="AF24" s="23"/>
-      <c r="AG24" s="11"/>
-      <c r="AH24" s="11"/>
-      <c r="AI24" s="23"/>
-    </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="19"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="19"/>
+    </row>
+    <row r="25" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
-      <c r="X25" s="23"/>
-      <c r="Y25" s="23"/>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="11"/>
-      <c r="AB25" s="23"/>
-      <c r="AC25" s="23"/>
-      <c r="AD25" s="23"/>
-      <c r="AE25" s="23"/>
-      <c r="AF25" s="23"/>
-      <c r="AG25" s="11"/>
-      <c r="AH25" s="11"/>
-      <c r="AI25" s="23"/>
-    </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="19"/>
+      <c r="AF25" s="19"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="19"/>
+    </row>
+    <row r="26" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="23"/>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="23"/>
-      <c r="AC26" s="23"/>
-      <c r="AD26" s="23"/>
-      <c r="AE26" s="23"/>
-      <c r="AF26" s="23"/>
-      <c r="AG26" s="11"/>
-      <c r="AH26" s="11"/>
-      <c r="AI26" s="23"/>
-    </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9" t="s">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="19"/>
+      <c r="AC26" s="19"/>
+      <c r="AD26" s="19"/>
+      <c r="AE26" s="19"/>
+      <c r="AF26" s="19"/>
+      <c r="AG26" s="7"/>
+      <c r="AH26" s="7"/>
+      <c r="AI26" s="19"/>
+    </row>
+    <row r="27" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B27" s="23"/>
+      <c r="C27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
-      <c r="AG27" s="11"/>
-      <c r="AH27" s="11"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
       <c r="AI27" s="2"/>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="18">
+    <row r="28" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="14">
         <f>SUM(E21:E27)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="14">
         <f t="shared" ref="F28:AH28" si="1">SUM(F21:F27)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L28" s="18">
+      <c r="L28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M28" s="18">
+      <c r="M28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N28" s="18">
+      <c r="N28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O28" s="18">
+      <c r="O28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P28" s="18">
+      <c r="P28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="18">
+      <c r="Q28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R28" s="18">
+      <c r="R28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S28" s="18">
+      <c r="S28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T28" s="18">
+      <c r="T28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U28" s="18">
+      <c r="U28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V28" s="18">
+      <c r="V28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W28" s="18">
+      <c r="W28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X28" s="18">
+      <c r="X28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y28" s="18">
+      <c r="Y28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z28" s="18">
+      <c r="Z28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA28" s="18">
+      <c r="AA28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="18">
+      <c r="AB28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="18">
+      <c r="AC28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AD28" s="18">
+      <c r="AD28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE28" s="18">
+      <c r="AE28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AF28" s="18">
+      <c r="AF28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="18">
+      <c r="AG28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AH28" s="18">
+      <c r="AH28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AI28" s="19"/>
-    </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="D30" s="20" t="s">
+      <c r="AI28" s="15"/>
+    </row>
+    <row r="30" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D30" s="16" t="s">
         <v>86</v>
       </c>
       <c r="E30">
@@ -3033,8 +3501,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.3">
-      <c r="D32" s="21" t="s">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="D32" s="17" t="s">
         <v>87</v>
       </c>
       <c r="F32">

</xml_diff>